<commit_message>
insert to db working
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\excel2DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5531B840-B0F7-42B6-B3FB-0385A55519F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B1AD04-D1F1-485C-BAEB-2044F0A25397}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="templete" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>fyit</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>varchar(40)</t>
   </si>
   <si>
@@ -121,12 +118,6 @@
     <t>sing</t>
   </si>
   <si>
-    <t xml:space="preserve">id </t>
-  </si>
-  <si>
-    <t>varchr(40)</t>
-  </si>
-  <si>
     <t>sheetName</t>
   </si>
   <si>
@@ -152,6 +143,12 @@
   </si>
   <si>
     <t>vijayd</t>
+  </si>
+  <si>
+    <t>varchar(300)</t>
+  </si>
+  <si>
+    <t>int (100)</t>
   </si>
 </sst>
 </file>
@@ -193,9 +190,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,24 +556,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -581,35 +581,35 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -617,41 +617,41 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -659,30 +659,30 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +705,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,10 +716,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,10 +727,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -754,82 +754,85 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
+      <c r="A1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>8422082978</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>8877559966</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>1111111111</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
+        <v>8422082778</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>8422082578</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C5">
-        <v>4444444444</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -852,16 +855,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,10 +872,10 @@
         <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>8422082989</v>
@@ -883,10 +886,10 @@
         <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>9819576818</v>
@@ -897,10 +900,10 @@
         <v>204</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>9769504786</v>
@@ -911,10 +914,10 @@
         <v>205</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
       </c>
       <c r="D5">
         <v>5477812568</v>

</xml_diff>

<commit_message>
table value cross check with datatype
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="templete" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>fyit</t>
   </si>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -523,7 +523,9 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -649,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -668,7 +670,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -679,7 +681,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>

</xml_diff>